<commit_message>
update view penilaian dan monev, update form input pakai choices-tags, update data seeder
</commit_message>
<xml_diff>
--- a/public/DataExcel/dosen.xlsx
+++ b/public/DataExcel/dosen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT SIPPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2EFAB8-473F-40F9-9030-E898C00C10E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2865C0-DE28-49B4-BEA1-CBED440C3E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="844">
   <si>
     <t>0020046406</t>
   </si>
@@ -1331,6 +1331,1236 @@
   </si>
   <si>
     <t>Ir. Hangrie Jimmy Namserna,M.Si</t>
+  </si>
+  <si>
+    <t>0011017703</t>
+  </si>
+  <si>
+    <t>0003067809</t>
+  </si>
+  <si>
+    <t>0001078107</t>
+  </si>
+  <si>
+    <t>0017088104</t>
+  </si>
+  <si>
+    <t>0001048201</t>
+  </si>
+  <si>
+    <t>0013028401</t>
+  </si>
+  <si>
+    <t>0031108301</t>
+  </si>
+  <si>
+    <t>0012028202</t>
+  </si>
+  <si>
+    <t>0030118004</t>
+  </si>
+  <si>
+    <t>0029078202</t>
+  </si>
+  <si>
+    <t>0003057705</t>
+  </si>
+  <si>
+    <t>0018017808</t>
+  </si>
+  <si>
+    <t>0019086909</t>
+  </si>
+  <si>
+    <t>0028118401</t>
+  </si>
+  <si>
+    <t>0029018404</t>
+  </si>
+  <si>
+    <t>0004097305</t>
+  </si>
+  <si>
+    <t>0022128004</t>
+  </si>
+  <si>
+    <t>0019107803</t>
+  </si>
+  <si>
+    <t>0015068104</t>
+  </si>
+  <si>
+    <t>0002116904</t>
+  </si>
+  <si>
+    <t>0024047801</t>
+  </si>
+  <si>
+    <t>0028127601</t>
+  </si>
+  <si>
+    <t>0007058401</t>
+  </si>
+  <si>
+    <t>0006127705</t>
+  </si>
+  <si>
+    <t>0006068003</t>
+  </si>
+  <si>
+    <t>0005037908</t>
+  </si>
+  <si>
+    <t>0020086507</t>
+  </si>
+  <si>
+    <t>0012127909</t>
+  </si>
+  <si>
+    <t>0006068301</t>
+  </si>
+  <si>
+    <t>0014067703</t>
+  </si>
+  <si>
+    <t>0003077403</t>
+  </si>
+  <si>
+    <t>0006076811</t>
+  </si>
+  <si>
+    <t>0023037905</t>
+  </si>
+  <si>
+    <t>0017088201</t>
+  </si>
+  <si>
+    <t>0007087603</t>
+  </si>
+  <si>
+    <t>0005037005</t>
+  </si>
+  <si>
+    <t>0027017904</t>
+  </si>
+  <si>
+    <t>0009067805</t>
+  </si>
+  <si>
+    <t>0017076911</t>
+  </si>
+  <si>
+    <t>0002017404</t>
+  </si>
+  <si>
+    <t>0011037803</t>
+  </si>
+  <si>
+    <t>0020086704</t>
+  </si>
+  <si>
+    <t>0007026704</t>
+  </si>
+  <si>
+    <t>0029115705</t>
+  </si>
+  <si>
+    <t>0009096403</t>
+  </si>
+  <si>
+    <t>0011066705</t>
+  </si>
+  <si>
+    <t>0017036209</t>
+  </si>
+  <si>
+    <t>0022116211</t>
+  </si>
+  <si>
+    <t>0030017705</t>
+  </si>
+  <si>
+    <t>0031057303</t>
+  </si>
+  <si>
+    <t>0030097606</t>
+  </si>
+  <si>
+    <t>0017077603</t>
+  </si>
+  <si>
+    <t>0025017704</t>
+  </si>
+  <si>
+    <t>0017107701</t>
+  </si>
+  <si>
+    <t>0004036805</t>
+  </si>
+  <si>
+    <t>0008067006</t>
+  </si>
+  <si>
+    <t>0027096909</t>
+  </si>
+  <si>
+    <t>0002107503</t>
+  </si>
+  <si>
+    <t>0010077903</t>
+  </si>
+  <si>
+    <t>0016066412</t>
+  </si>
+  <si>
+    <t>0024106005</t>
+  </si>
+  <si>
+    <t>0029026804</t>
+  </si>
+  <si>
+    <t>0002036703</t>
+  </si>
+  <si>
+    <t>0016026311</t>
+  </si>
+  <si>
+    <t>0008076005</t>
+  </si>
+  <si>
+    <t>0019076105</t>
+  </si>
+  <si>
+    <t>0029126503</t>
+  </si>
+  <si>
+    <t>0030046009</t>
+  </si>
+  <si>
+    <t>0013016304</t>
+  </si>
+  <si>
+    <t>0016116604</t>
+  </si>
+  <si>
+    <t>0006016905</t>
+  </si>
+  <si>
+    <t>0030036304</t>
+  </si>
+  <si>
+    <t>0007086407</t>
+  </si>
+  <si>
+    <t>0024036705</t>
+  </si>
+  <si>
+    <t>0017046410</t>
+  </si>
+  <si>
+    <t>0004046414</t>
+  </si>
+  <si>
+    <t>0012095910</t>
+  </si>
+  <si>
+    <t>0007026208</t>
+  </si>
+  <si>
+    <t>0004056210</t>
+  </si>
+  <si>
+    <t>0012046013</t>
+  </si>
+  <si>
+    <t>0023126408</t>
+  </si>
+  <si>
+    <t>0003106405</t>
+  </si>
+  <si>
+    <t>0023028201</t>
+  </si>
+  <si>
+    <t>0003067405</t>
+  </si>
+  <si>
+    <t>0010097404</t>
+  </si>
+  <si>
+    <t>0023057303</t>
+  </si>
+  <si>
+    <t>0020017405</t>
+  </si>
+  <si>
+    <t>0005117505</t>
+  </si>
+  <si>
+    <t>0003036905</t>
+  </si>
+  <si>
+    <t>0024108205</t>
+  </si>
+  <si>
+    <t>0014118402</t>
+  </si>
+  <si>
+    <t>0011118504</t>
+  </si>
+  <si>
+    <t>0018058502</t>
+  </si>
+  <si>
+    <t>0021077903</t>
+  </si>
+  <si>
+    <t>0013076705</t>
+  </si>
+  <si>
+    <t>0006028401</t>
+  </si>
+  <si>
+    <t>0015078305</t>
+  </si>
+  <si>
+    <t>0029117301</t>
+  </si>
+  <si>
+    <t>0006048403</t>
+  </si>
+  <si>
+    <t>0029107301</t>
+  </si>
+  <si>
+    <t>0022097602</t>
+  </si>
+  <si>
+    <t>0014038103</t>
+  </si>
+  <si>
+    <t>0023017803</t>
+  </si>
+  <si>
+    <t>0030097705</t>
+  </si>
+  <si>
+    <t>0012127208</t>
+  </si>
+  <si>
+    <t>0025048202</t>
+  </si>
+  <si>
+    <t>0009127504</t>
+  </si>
+  <si>
+    <t>0017096012</t>
+  </si>
+  <si>
+    <t>0030085601</t>
+  </si>
+  <si>
+    <t>0018046605</t>
+  </si>
+  <si>
+    <t>0003036510</t>
+  </si>
+  <si>
+    <t>0018046409</t>
+  </si>
+  <si>
+    <t>0019085708</t>
+  </si>
+  <si>
+    <t>0002116006</t>
+  </si>
+  <si>
+    <t>0008096205</t>
+  </si>
+  <si>
+    <t>0014046604</t>
+  </si>
+  <si>
+    <t>0020046407</t>
+  </si>
+  <si>
+    <t>0023096310</t>
+  </si>
+  <si>
+    <t>0026035708</t>
+  </si>
+  <si>
+    <t>0010056007</t>
+  </si>
+  <si>
+    <t>0008065804</t>
+  </si>
+  <si>
+    <t>0014076508</t>
+  </si>
+  <si>
+    <t>0018086206</t>
+  </si>
+  <si>
+    <t>0004076506</t>
+  </si>
+  <si>
+    <t>0023106702</t>
+  </si>
+  <si>
+    <t>0003096006</t>
+  </si>
+  <si>
+    <t>0023046206</t>
+  </si>
+  <si>
+    <t>0005076606</t>
+  </si>
+  <si>
+    <t>0008086810</t>
+  </si>
+  <si>
+    <t>0010067507</t>
+  </si>
+  <si>
+    <t>0029017303</t>
+  </si>
+  <si>
+    <t>0007068105</t>
+  </si>
+  <si>
+    <t>0023017703</t>
+  </si>
+  <si>
+    <t>0010027806</t>
+  </si>
+  <si>
+    <t>0023098001</t>
+  </si>
+  <si>
+    <t>0028068005</t>
+  </si>
+  <si>
+    <t>0024116904</t>
+  </si>
+  <si>
+    <t>0021107609</t>
+  </si>
+  <si>
+    <t>0028018107</t>
+  </si>
+  <si>
+    <t>0015127206</t>
+  </si>
+  <si>
+    <t>0022027603</t>
+  </si>
+  <si>
+    <t>0009098201</t>
+  </si>
+  <si>
+    <t>0016107604</t>
+  </si>
+  <si>
+    <t>0021017904</t>
+  </si>
+  <si>
+    <t>002345780</t>
+  </si>
+  <si>
+    <t>0026037106</t>
+  </si>
+  <si>
+    <t>0011098102</t>
+  </si>
+  <si>
+    <t>0016098303</t>
+  </si>
+  <si>
+    <t>0031126919</t>
+  </si>
+  <si>
+    <t>0005048501</t>
+  </si>
+  <si>
+    <t>0003038003</t>
+  </si>
+  <si>
+    <t>0026118001</t>
+  </si>
+  <si>
+    <t>0018038201</t>
+  </si>
+  <si>
+    <t>0029098102</t>
+  </si>
+  <si>
+    <t>0002058202</t>
+  </si>
+  <si>
+    <t>0021018601</t>
+  </si>
+  <si>
+    <t>0009018202</t>
+  </si>
+  <si>
+    <t>0003058007</t>
+  </si>
+  <si>
+    <t>0027107604</t>
+  </si>
+  <si>
+    <t>0023117703</t>
+  </si>
+  <si>
+    <t>0026108301</t>
+  </si>
+  <si>
+    <t>0008118202</t>
+  </si>
+  <si>
+    <t>0016117904</t>
+  </si>
+  <si>
+    <t>0030107502</t>
+  </si>
+  <si>
+    <t>0002047903</t>
+  </si>
+  <si>
+    <t>0025096312</t>
+  </si>
+  <si>
+    <t>0006127302</t>
+  </si>
+  <si>
+    <t>0018056509</t>
+  </si>
+  <si>
+    <t>0012086809</t>
+  </si>
+  <si>
+    <t>0023076106</t>
+  </si>
+  <si>
+    <t>0008086809</t>
+  </si>
+  <si>
+    <t>0006105808</t>
+  </si>
+  <si>
+    <t>0028086604</t>
+  </si>
+  <si>
+    <t>0012108007</t>
+  </si>
+  <si>
+    <t>0012128301</t>
+  </si>
+  <si>
+    <t>0005038601</t>
+  </si>
+  <si>
+    <t>0002087908</t>
+  </si>
+  <si>
+    <t>0015127901</t>
+  </si>
+  <si>
+    <t>0014108602</t>
+  </si>
+  <si>
+    <t>0008057903</t>
+  </si>
+  <si>
+    <t>0024058501</t>
+  </si>
+  <si>
+    <t>0016077802</t>
+  </si>
+  <si>
+    <t>0016086804</t>
+  </si>
+  <si>
+    <t>0004117404</t>
+  </si>
+  <si>
+    <t>0023117204</t>
+  </si>
+  <si>
+    <t>0020038205</t>
+  </si>
+  <si>
+    <t>0029087702</t>
+  </si>
+  <si>
+    <t>0011017413</t>
+  </si>
+  <si>
+    <t>0031128006</t>
+  </si>
+  <si>
+    <t>0003107706</t>
+  </si>
+  <si>
+    <t>0004077306</t>
+  </si>
+  <si>
+    <t>0009077804</t>
+  </si>
+  <si>
+    <t>0001057909</t>
+  </si>
+  <si>
+    <t>0027117801</t>
+  </si>
+  <si>
+    <t>0021037802</t>
+  </si>
+  <si>
+    <t>0022048102</t>
+  </si>
+  <si>
+    <t>0019027502</t>
+  </si>
+  <si>
+    <t>0004106404</t>
+  </si>
+  <si>
+    <t>0010067906</t>
+  </si>
+  <si>
+    <t>0015067804</t>
+  </si>
+  <si>
+    <t>0001077508</t>
+  </si>
+  <si>
+    <t>0029057603</t>
+  </si>
+  <si>
+    <t>0022058103</t>
+  </si>
+  <si>
+    <t>0020038202</t>
+  </si>
+  <si>
+    <t>Abdul Rahman Ollong, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Abraham William Manumpil, S.Ik.,M.Si</t>
+  </si>
+  <si>
+    <t>Aditya Rahmadaniarti, S.Hut.,M.Sc</t>
+  </si>
+  <si>
+    <t>Alexander Rumatora, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Alfredo Otto Wanma, S.Hut.,M.Si</t>
+  </si>
+  <si>
+    <t>Alnita Baaka, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Amilda Auri, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Ana Tampang, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Angelina Novita Tethool, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anik Wuriasih, SE, M.Si.Ak,CA </t>
+  </si>
+  <si>
+    <t>Anjeli Sulistianti Paisey, S.Pi,M.Si</t>
+  </si>
+  <si>
+    <t>Baso Daeng, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Besse Amriati, SP, MP</t>
+  </si>
+  <si>
+    <t>Camelia Lusandri Numberi, SE.,M.Sc</t>
+  </si>
+  <si>
+    <t>Charly Bravo Wanggai, ST, M.I.L</t>
+  </si>
+  <si>
+    <t>Christian Soleman Imburi, S.Hut.,M.Sc</t>
+  </si>
+  <si>
+    <t>Daniel Yohanis Seseray, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Danny Erlis Waimbo, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Dedi Parenden, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>DedY Riantoro, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Deny A. Iyai, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Desni T.Ruli Saragih, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Devi Manuhua, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Diana Sawen, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Dina Arung Padang, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Dirarini Sudarwadi, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Djumiati Mustiah, SP, M.P</t>
+  </si>
+  <si>
+    <t>Dominggas M.H. Renwarin, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Donny Aristone Djitmau, S.Hut.,M.Sc</t>
+  </si>
+  <si>
+    <t>Dougklas Ledrik Wattimury, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Abdul Azis, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>DR. Abdul Hamid A.Toha, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Agustinus Murdjoko, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Albertus Girik Allo, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Alce Ilona Noya, SP.,M.Si</t>
+  </si>
+  <si>
+    <t>DR. Alianto, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Anton Silas Sinery, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Antoni Ungirwalu, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Cicilia M.E. Susanti, S.Hut,M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Emmanuel Manangkalangi,S.Pi.,M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Gandi Yantri S. Purba, M.Si</t>
+  </si>
+  <si>
+    <t>DR. Ir. Elfira Kariane Suawa, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Freddy Pattiselano, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Irba Unggul Warsono, MP</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Irnanda A.F. Djuuna, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Mohamad Jen Wajo, MP</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Onesimus Yoku, MS</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Sientje Daisy Rumetor, MP</t>
+  </si>
+  <si>
+    <t>Dr. Mahmud, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Muhammad G.Tafalas, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Renny Purnawati, S.Hut.,M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Selvi Tebaiy, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Sepus Marten Fatem, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr. Stepanus Pakage, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Dr. Syafrudin Raharjo, S.Pi, MT</t>
+  </si>
+  <si>
+    <t>Dr. Yuanike, S.Si, M.Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr.Alusius P.E.Widodo, S.Pt, M.Sc.Ag   </t>
+  </si>
+  <si>
+    <t>Dr.drh. Priyo Sambodo, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Elieser Y.I.V. Sirami, S.Hut.,M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Antonius Suparno, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Bambang Nugroho, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Eko Agus Martanto, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Ihwan Tjolli, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Ishak Musa'ad, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Julius Dwi Nugroho, M.Sc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr.Ir. Marlyn N. Lekitoo, MS        </t>
+  </si>
+  <si>
+    <t>Dr.Ir. Martha Kayadoe, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Muhammad Affan Mu'in, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Mulyadi, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Nouke Lenda Mawikere, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Nurhaidah I. Sinaga, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Paulus Boli, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Reymas M.R. Ruimassa,M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Ridwan Sala, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Rudy A. Maturbongs, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Rully Novie Wurarah, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Samen Baan, MP</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Sangle Yohanes Randa, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Saraswati Prabawardani,M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Sintje Lumatauw, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Soetjipto Moeljono, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ir. Vera Sabariah, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Jimmy Frans Wanma, S.Hut, M.App.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Jonni Marwa, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Ludia Th. Wambrauw,SP, M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Rima H.S. Siburian, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Dr.Selmi Dedi, SE, M.AB</t>
+  </si>
+  <si>
+    <t>Dr.Thomas Frans Pattiasina,S.Pi,M.Sc</t>
+  </si>
+  <si>
+    <t>Dr.Trisiwi W. Widayati, S.Pt, MM</t>
+  </si>
+  <si>
+    <t>drh. Dwi Nurhayati.,M.Sc</t>
+  </si>
+  <si>
+    <t>drh. Isti Widayati, M.Sc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drh. Noviyanti, MPH </t>
+  </si>
+  <si>
+    <t>Evelin Anggelina Tanur, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Fadli Zainuddin, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Fanny F.C. Simatauw, S.Pi, MP</t>
+  </si>
+  <si>
+    <t>Ferawati Runtuboi,S.Ik , M.Si</t>
+  </si>
+  <si>
+    <t>Fitriyah Irmawati E.S, ST, M.Si</t>
+  </si>
+  <si>
+    <t>Francina F. Kesaulia, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Frida Aprilia Loinenak, S.Ik, M.Si</t>
+  </si>
+  <si>
+    <t>Hans F.Z. Peday, S.Hut , M.Si</t>
+  </si>
+  <si>
+    <t>Hendrik Victor Ayhuan, S.Ik.,M.Si</t>
+  </si>
+  <si>
+    <t>Herman Wafom Tubur, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Hermanus Warmetan, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Hieronymus Y.Chrysostomus, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Hotlan Manik, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Hustianto Sudarwadi, SE, MSc</t>
+  </si>
+  <si>
+    <t>Ida Lapadi, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Ir. A. Gatot Murwanto, M.Si</t>
+  </si>
+  <si>
+    <t>Ir. Albert W.A. Renyaan, MP</t>
+  </si>
+  <si>
+    <t>Ir. B.M.G. Sadsoeitoeboen, M.Sc</t>
+  </si>
+  <si>
+    <t>Ir. B.Wahyuni I. Rahayu, MP</t>
+  </si>
+  <si>
+    <t>Ir. Bambang Tj. Hariadi, MP</t>
+  </si>
+  <si>
+    <t>Ir. Bernadus B. Rettob, M.Si</t>
+  </si>
+  <si>
+    <t>Ir. Djonli Woran, MP</t>
+  </si>
+  <si>
+    <t>Ir. Dwi Djoko Raharjo, MP</t>
+  </si>
+  <si>
+    <t>Ir. Endra Gunawan, MP</t>
+  </si>
+  <si>
+    <t>Ir. Erlina R. Situmorang, M.Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ir. Hanike Monim, M.Sc, Ph.D </t>
+  </si>
+  <si>
+    <t>Ir. Jacobus Wanggai, MP</t>
+  </si>
+  <si>
+    <t>Ir. Lambert N. Nuhuyanan,MP</t>
+  </si>
+  <si>
+    <t>Ir. Max Jundodago Tokede, MS</t>
+  </si>
+  <si>
+    <t>Ir. Mudjirahayu, M.Sc</t>
+  </si>
+  <si>
+    <t>Ir. Muhammad Djunaidi, M.Si</t>
+  </si>
+  <si>
+    <t>Ir. Muhammad Takdir, MP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ir. Obed Nedjo Lense, M.Sc, PhD </t>
+  </si>
+  <si>
+    <t>Ir. Rusdi Angrianto, MP</t>
+  </si>
+  <si>
+    <t>Ir. Susilo Budi Husodo, MP</t>
+  </si>
+  <si>
+    <t>Ir. Yosias Gandhi, M.Sc</t>
+  </si>
+  <si>
+    <t>Ir.Agustina Y.S. Arobaya, M.Sc</t>
+  </si>
+  <si>
+    <t>Iriani Sumpe, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Jafry Ferdinand Manuhutu, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Jein Sriana Toyib, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Jemmy Manan,S.Ik,DEA</t>
+  </si>
+  <si>
+    <t>Johan Fredrik Koibur, S.Pt, M.Si</t>
+  </si>
+  <si>
+    <t>Johanes Paulus Koromath, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>John Arnold Palulungan, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Johny Aninam, SE.,ME</t>
+  </si>
+  <si>
+    <t>Juliana Leiwakabessy, S.Pi, M,.Si</t>
+  </si>
+  <si>
+    <t>Ketysia Imelda Tewernusa, SE, M.Si</t>
+  </si>
+  <si>
+    <t>La Ode Alisyah, SE, M.Ec.Dev</t>
+  </si>
+  <si>
+    <t>Lilyani Margaretha Orisu, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Louis Soemadi Bopeng, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Lukas Yowel Sonbait, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Luky Sembel, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Lutfi, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Magriet Ester Sawaki, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Makarius Bajari, SE, M.M</t>
+  </si>
+  <si>
+    <t>Marcus Ronaldo Maspaitella, S.P.,M.AgriComm</t>
+  </si>
+  <si>
+    <t>Margareth Sylvia Sabarofek,SE.,M.Si</t>
+  </si>
+  <si>
+    <t>Marhan, S.Pi, MT</t>
+  </si>
+  <si>
+    <t>Maria Magdalena Semet, S.E, M.Sc</t>
+  </si>
+  <si>
+    <t>Mariana Hermina Peday, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Marlina Malino, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Martha A.C. Kareth, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Matheus Beljai, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Meliza Sartje Worabai, S.Si, M.Si</t>
+  </si>
+  <si>
+    <t>Mona Permatasari Mokodompit, SE,Ak.M.Ak</t>
+  </si>
+  <si>
+    <t>Muliyana Arifuddin, S.Hut, M.Wood,Sc</t>
+  </si>
+  <si>
+    <t>Mus Mualim, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Naftali Mansim, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Novita Panambe, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Nunang Lamaek May, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Nurhani Widiastuti, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Nurlaela, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Nurwidianto, SE.,M.Sc</t>
+  </si>
+  <si>
+    <t>Petrus Abraham Dimara, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Ir. Barahima, M.Si</t>
+  </si>
+  <si>
+    <t>Prof. Dr.Charly D. Heatubun, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Prof. Dr.Ir. Andoyo Supriyantono, M.Sc</t>
+  </si>
+  <si>
+    <t>Prof. Dr.Ir. Budi Santoso, MP</t>
+  </si>
+  <si>
+    <t>Prof. Dr.Ir. Sri Hartini, M.Sc</t>
+  </si>
+  <si>
+    <t>Prof. Dr.Ir. Wahyudi, M.Wood. Sc</t>
+  </si>
+  <si>
+    <t>Prof.Dr.Ir. Jacob Manusawai, M.H</t>
+  </si>
+  <si>
+    <t>Prof.Ir. Ricardo F. Tapilatu, M.Si.Ph.D</t>
+  </si>
+  <si>
+    <t>Purwaningsih, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Reinardus Liborius, S.Hut.,M.Sc</t>
+  </si>
+  <si>
+    <t>Rina Nelly Jowei, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Rintar Agus Simatupang, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Rizald Husein, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Rizki Arizona, S.Pt, M.Sc</t>
+  </si>
+  <si>
+    <t>Rumas Alma Yap, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Sarah Usman, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Sarce Babra Awom, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Selfanie Talakua, S.Pi.,M.Si</t>
+  </si>
+  <si>
+    <t>Simon P.O. Leatemia, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Simson Werimon, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Sisilia Maria Parinusa, S.P.,M.Si</t>
+  </si>
+  <si>
+    <t>Siti Aisah Bauw, SE, M.Sc</t>
+  </si>
+  <si>
+    <t>Srihartati Harto, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Suhaemi, S.Ik.,M.Si</t>
+  </si>
+  <si>
+    <t>Susanti Tasik, S.Hut, M.Biotech</t>
+  </si>
+  <si>
+    <t>Syarifuddin, SE, AK, M.Si</t>
+  </si>
+  <si>
+    <t>Ted Matheus Suruan, SE., M.Si</t>
+  </si>
+  <si>
+    <t>Tresia Sonya Tururaja,S.IK.,M.Si</t>
+  </si>
+  <si>
+    <t>Victor Rumere, SE,M.Si</t>
+  </si>
+  <si>
+    <t>Wolfram Yahya Mofu, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>Yafed Muyam, SP, M.Si</t>
+  </si>
+  <si>
+    <t>Yehiel H. Dasmasela, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Yohanes Y. Rahawarin, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Yori Turu Toja, S.Pi, M.Si</t>
+  </si>
+  <si>
+    <t>Yubelince Y. Runtuboi, S.Hut, M.Sc</t>
+  </si>
+  <si>
+    <t>Yulius Heri Saptomo, SE, M.Si</t>
+  </si>
+  <si>
+    <t>Yuyu Rahayu, S.Hut, M,Sc</t>
+  </si>
+  <si>
+    <t>Yuyun Puji Rahayu, S.P, M.Dev.Eco (Adv)</t>
+  </si>
+  <si>
+    <t>Zulfikar Mardiyadi, S.Hut, M.Si</t>
+  </si>
+  <si>
+    <t>0005018107</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16483FC-62EB-4506-A3E1-D0D0FD970BC9}">
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F349" sqref="F349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4125,6 +5355,2261 @@
         <v>29</v>
       </c>
     </row>
+    <row r="218" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="C218">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="C219">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="C220">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="C221">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="C222">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C223">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="C224">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="C225">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="C226">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="C227">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A228" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="C228">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="C229">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C230">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="C231">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C232">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="C233">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="C234">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="C235">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="C236">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C237">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="C238">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="C239">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="C240">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="C241">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="C242">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="C243">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="C244">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="C245">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C246">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C247">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="C248">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="C249">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B250" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="C250">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="C251">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="C252">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C253">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A254" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="C254">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="C255">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="C256">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="C257">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="C258">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A259" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="C259">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="C260">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C261">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="C262">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="C263">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C264">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A265" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="C265">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="C266">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="C267">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B268" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="C268">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="C269">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="C270">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C271">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="C272">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="C273">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="C274">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="C275">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C276">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A277" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="C277">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A278" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="C278">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A279" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="C279">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A280" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="C280">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A281" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="C281">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A282" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="C282">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A283" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="C283">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="C284">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A285" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B285" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="C285">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A286" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B286" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="C286">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B287" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="C287">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A288" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="B288" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="C288">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A289" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B289" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="C289">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A290" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="B290" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="C290">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C291">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="C292">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B293" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="C293">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="C294">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C295">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C296">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B297" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="C297">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B298" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="C298">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="C299">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="B300" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="C300">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="C301">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="B302" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="C302">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="C303">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="C304">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B305" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="C305">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B306" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="C306">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B307" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="C307">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="C308">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="C309">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="C310">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B311" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C311">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B312" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C312">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B313" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="C313">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B314" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C314">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B315" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="C315">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B316" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="C316">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B317" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="C317">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B318" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="C318">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B319" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="C319">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B320" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="C320">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B321" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="C321">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B322" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="C322">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B323" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="C323">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B324" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="C324">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A325" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B325" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="C325">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A326" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B326" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="C326">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="B327" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="C327">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B328" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="C328">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B329" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C329">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B330" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="C330">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B331" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C331">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B332" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="C332">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="B333" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="C333">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>754</v>
+      </c>
+      <c r="C334">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B335" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C335">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="B336" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="C336">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B337" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="C337">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="B338" s="4" t="s">
+        <v>758</v>
+      </c>
+      <c r="C338">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="B339" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="C339">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A340" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B340" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C340">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A341" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="B341" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="C341">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B342" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C342">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B343" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="C343">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="B344" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="C344">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B345" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="C345">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="B346" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="C346">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="B347" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="C347">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B348" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="C348">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A349" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B349" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="C349">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A350" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="B350" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="C350">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="B351" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="C351">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="B352" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="C352">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="B353" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="C353">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B354" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="C354">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="B355" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="C355">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="C356">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="C357">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="C358">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="B359" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="C359">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="C360">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C361">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="B362" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="C362">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="C363">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="C364">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A365" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B365" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="C365">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A366" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="B366" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="C366">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A367" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="B367" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="C367">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A368" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="B368" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="C368">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A369" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="B369" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="C369">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A370" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="B370" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="C370">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A371" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="B371" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="C371">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A372" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B372" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="C372">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A373" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="B373" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C373">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A374" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="B374" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="C374">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A375" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="B375" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="C375">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A376" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="B376" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="C376">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A377" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B377" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="C377">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A378" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="B378" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="C378">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A379" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B379" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="C379">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A380" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="B380" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="C380">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A381" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B381" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="C381">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A382" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="B382" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="C382">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A383" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B383" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="C383">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A384" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="B384" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="C384">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A385" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B385" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="C385">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A386" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B386" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="C386">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A387" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="B387" s="4" t="s">
+        <v>807</v>
+      </c>
+      <c r="C387">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A388" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="B388" s="4" t="s">
+        <v>808</v>
+      </c>
+      <c r="C388">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A389" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="B389" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="C389">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A390" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="B390" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="C390">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A391" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B391" s="4" t="s">
+        <v>811</v>
+      </c>
+      <c r="C391">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A392" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="B392" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="C392">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A393" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="B393" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="C393">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A394" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="B394" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="C394">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A395" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B395" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="C395">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A396" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="B396" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="C396">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A397" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B397" s="4" t="s">
+        <v>817</v>
+      </c>
+      <c r="C397">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A398" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="B398" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="C398">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A399" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B399" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="C399">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A400" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B400" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="C400">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A401" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B401" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="C401">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A402" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B402" s="4" t="s">
+        <v>822</v>
+      </c>
+      <c r="C402">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A403" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B403" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="C403">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A404" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="B404" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="C404">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A405" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B405" s="4" t="s">
+        <v>825</v>
+      </c>
+      <c r="C405">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A406" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B406" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="C406">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A407" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="B407" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C407">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B408" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="C408">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A409" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="B409" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="C409">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A410" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="C410">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A411" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="B411" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="C411">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="B412" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="C412">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A413" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B413" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="C413">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A414" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="B414" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C414">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A415" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B415" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="C415">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A416" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="B416" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="C416">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A417" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B417" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="C417">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A418" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B418" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="C418">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A419" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B419" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="C419">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A420" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="B420" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="C420">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A421" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B421" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="C421">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A422" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B422" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="C422">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1.88" right="0.51181102362204722" top="0.74803149606299213" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="80" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update email di file .env, update view datatables kegiatan, update kolom table publikasi
</commit_message>
<xml_diff>
--- a/public/DataExcel/dosen.xlsx
+++ b/public/DataExcel/dosen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT SIPPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2865C0-DE28-49B4-BEA1-CBED440C3E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA998DFC-A77A-48F3-8050-21A35BA20ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dosen" sheetId="15" r:id="rId1"/>
@@ -2957,7 +2957,7 @@
   <dimension ref="A1:C422"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F349" sqref="F349"/>
+      <selection activeCell="B348" sqref="B348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>